<commit_message>
Update Add and Search
-Sửa type của DOB, StartDate, EndDate từ "text" sang "date"
-Sửa tài liệu TestCase: Xóa phần kiểm tra lỗi của DOB, StartDate,
EndDate
</commit_message>
<xml_diff>
--- a/docs/CMS_TestCase_V1.0.xlsx
+++ b/docs/CMS_TestCase_V1.0.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Win8.1 VS10 X64\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bachc_000\Documents\GitHub\CustomerManager\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -309,7 +309,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="139">
   <si>
     <t>Back to TestReport</t>
   </si>
@@ -517,26 +517,6 @@
     <t>Kiểm tra giá trị Income không phải là số thực</t>
   </si>
   <si>
-    <t>Hiển thị cảnh báo "Date error"</t>
-  </si>
-  <si>
-    <t>1. Nhập ngày, tháng, năm không đúng tiêu chuẩn vào DOB, Start Date, End Date 
-2. Bấm nút Add</t>
-  </si>
-  <si>
-    <t>Kiểm tra ngày nhập không đúng tiêu chuẩn ngày tháng</t>
-  </si>
-  <si>
-    <t>Hiển thị cảnh báo "Date must be in the format dd/mm/yyyy"</t>
-  </si>
-  <si>
-    <t>1. Nhập ngày theo định dạng khác dd/mm/yyyy vào DOB, Start Date, End Date 
-2. Bấm nút Add</t>
-  </si>
-  <si>
-    <t>Kiểm tra ngày không phải định dạng ngày dd/mm/yyyy</t>
-  </si>
-  <si>
     <t>Hiển thị cảnh báo "Start date in must before End date"</t>
   </si>
   <si>
@@ -699,14 +679,6 @@
 2. Bấm nút Update</t>
   </si>
   <si>
-    <t>1. Nhập ngày, tháng, năm không đúng tiêu chuẩn vào DOB, Start Date, End Date 
-2. Bấm nút Update</t>
-  </si>
-  <si>
-    <t>1. Nhập ngày theo định dạng khác dd/mm/yyyy vào DOB, Start Date, End Date 
-2. Bấm nút Update</t>
-  </si>
-  <si>
     <t>1. Nhập ngày Start Date sau ngày End Date 
 2. Bấm nút Update</t>
   </si>
@@ -778,6 +750,9 @@
   </si>
   <si>
     <t>Add customer maintain test</t>
+  </si>
+  <si>
+    <t>05/15/2015</t>
   </si>
 </sst>
 </file>
@@ -1343,6 +1318,66 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1354,66 +1389,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1855,8 +1830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2378,13 +2353,13 @@
     <row r="2" spans="1:7" s="19" customFormat="1" ht="75.75" customHeight="1">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="21"/>
@@ -2395,54 +2370,54 @@
       <c r="B4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="55" t="s">
-        <v>139</v>
-      </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
+      <c r="C4" s="75" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
       <c r="F4" s="23" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1">
       <c r="B5" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="55" t="s">
-        <v>141</v>
-      </c>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
+      <c r="C5" s="75" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
       <c r="F5" s="23" t="s">
         <v>17</v>
       </c>
       <c r="G5" s="24"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="57" t="str">
+      <c r="C6" s="77" t="str">
         <f>C5&amp;"_"&amp;"TEST"&amp;"_"&amp;"v1.0"</f>
         <v>CMS_TEST_v1.0</v>
       </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
       <c r="F6" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="77">
+      <c r="G6" s="73">
         <v>42252</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="13.5" customHeight="1">
-      <c r="B7" s="56"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
       <c r="F7" s="23" t="s">
         <v>22</v>
       </c>
@@ -2489,39 +2464,43 @@
       </c>
     </row>
     <row r="12" spans="1:7" s="38" customFormat="1">
-      <c r="B12" s="77">
+      <c r="B12" s="73">
         <v>42252</v>
       </c>
       <c r="C12" s="39"/>
       <c r="D12" s="40"/>
       <c r="E12" s="40" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F12" s="41" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="G12" s="42"/>
     </row>
     <row r="13" spans="1:7" s="38" customFormat="1" ht="21.75" customHeight="1">
-      <c r="B13" s="77">
+      <c r="B13" s="73">
         <v>42252</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="40"/>
       <c r="E13" s="40" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F13" s="40" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="G13" s="44"/>
     </row>
     <row r="14" spans="1:7" s="38" customFormat="1" ht="19.5" customHeight="1">
-      <c r="B14" s="43"/>
+      <c r="B14" s="73" t="s">
+        <v>138</v>
+      </c>
       <c r="C14" s="39"/>
       <c r="D14" s="40"/>
       <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
+      <c r="F14" s="40" t="s">
+        <v>137</v>
+      </c>
       <c r="G14" s="44"/>
     </row>
     <row r="15" spans="1:7" s="38" customFormat="1" ht="21.75" customHeight="1">
@@ -3230,450 +3209,406 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I172"/>
+  <dimension ref="A1:I170"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A5" sqref="A5:A18"/>
       <selection pane="topRight" activeCell="A5" sqref="A5:A18"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5:A18"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5:A18"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="58" customWidth="1"/>
-    <col min="2" max="2" width="32.875" style="58" customWidth="1"/>
-    <col min="3" max="3" width="14.25" style="58" customWidth="1"/>
-    <col min="4" max="4" width="39.875" style="58" customWidth="1"/>
-    <col min="5" max="5" width="37.25" style="58" customWidth="1"/>
-    <col min="6" max="6" width="10.5" style="58" customWidth="1"/>
-    <col min="7" max="7" width="11.875" style="58" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="58"/>
+    <col min="1" max="1" width="14.5" style="54" customWidth="1"/>
+    <col min="2" max="2" width="32.875" style="54" customWidth="1"/>
+    <col min="3" max="3" width="14.25" style="54" customWidth="1"/>
+    <col min="4" max="4" width="39.875" style="54" customWidth="1"/>
+    <col min="5" max="5" width="37.25" style="54" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="54" customWidth="1"/>
+    <col min="7" max="7" width="11.875" style="54" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="76"/>
+      <c r="C1" s="72"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="75"/>
+      <c r="F1" s="71"/>
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
     </row>
     <row r="2" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="74" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="73" t="str">
-        <f>"Pass: "&amp;COUNTIF($G$5:$G$936,"Pass")</f>
-        <v>Pass: 14</v>
-      </c>
-      <c r="D2" s="73" t="str">
-        <f>"Fail: "&amp;COUNTIF($G$5:$G$936,"Fail")</f>
+      <c r="B2" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="69" t="str">
+        <f>"Pass: "&amp;COUNTIF($G$5:$G$934,"Pass")</f>
+        <v>Pass: 12</v>
+      </c>
+      <c r="D2" s="69" t="str">
+        <f>"Fail: "&amp;COUNTIF($G$5:$G$934,"Fail")</f>
         <v>Fail: 0</v>
       </c>
-      <c r="E2" s="71" t="str">
-        <f>"N/A: "&amp;COUNTIF($G$5:$G$936,"N/A")</f>
+      <c r="E2" s="67" t="str">
+        <f>"N/A: "&amp;COUNTIF($G$5:$G$934,"N/A")</f>
         <v>N/A: 0</v>
       </c>
-      <c r="F2" s="71"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="62"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="58"/>
     </row>
     <row r="3" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="72" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="70" t="str">
-        <f>"Number of cases: "&amp;(COUNTA($A$5:$A$936))</f>
-        <v>Number of cases: 14</v>
-      </c>
-      <c r="D3" s="71" t="str">
-        <f>"Untested: "&amp;COUNTIF($G$5:$G$936,"Untest")</f>
+      <c r="B3" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="66" t="str">
+        <f>"Number of cases: "&amp;(COUNTA($A$5:$A$934))</f>
+        <v>Number of cases: 12</v>
+      </c>
+      <c r="D3" s="67" t="str">
+        <f>"Untested: "&amp;COUNTIF($G$5:$G$934,"Untest")</f>
         <v>Untested: 0</v>
       </c>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="62"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="58"/>
     </row>
     <row r="4" spans="1:9" ht="28.35" customHeight="1">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="67" t="s">
+      <c r="D4" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="67" t="s">
+      <c r="E4" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="68" t="s">
-        <v>94</v>
-      </c>
-      <c r="G4" s="67" t="s">
+      <c r="F4" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="67" t="s">
+      <c r="H4" s="63" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="66" customFormat="1" ht="21">
-      <c r="A5" s="64" t="str">
-        <f>IF(OR(B5&lt;&gt;"",E5&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+    <row r="5" spans="1:9" s="62" customFormat="1" ht="21">
+      <c r="A5" s="60" t="str">
+        <f t="shared" ref="A5:A16" si="0">IF(OR(B5&lt;&gt;"",E5&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
         <v>[Add Customer-1]</v>
       </c>
-      <c r="B5" s="64" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" s="64" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5" s="64" t="s">
-        <v>90</v>
-      </c>
-      <c r="F5" s="65"/>
-      <c r="G5" s="61" t="s">
+      <c r="B5" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="60" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="61"/>
+      <c r="G5" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="60">
+      <c r="H5" s="56">
         <v>42133</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="21">
-      <c r="A6" s="64" t="str">
-        <f>IF(OR(B6&lt;&gt;"",E6&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+      <c r="A6" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Add Customer-2]</v>
       </c>
-      <c r="B6" s="64" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64" t="s">
-        <v>88</v>
-      </c>
-      <c r="E6" s="64" t="s">
-        <v>87</v>
-      </c>
-      <c r="F6" s="65"/>
-      <c r="G6" s="61" t="s">
+      <c r="B6" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="61"/>
+      <c r="G6" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="60">
+      <c r="H6" s="56">
         <v>42133</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="21">
-      <c r="A7" s="64" t="str">
-        <f>IF(OR(B7&lt;&gt;"",E7&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+      <c r="A7" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Add Customer-3]</v>
       </c>
-      <c r="B7" s="64" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="F7" s="65"/>
-      <c r="G7" s="61" t="s">
+      <c r="B7" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="61"/>
+      <c r="G7" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="60">
+      <c r="H7" s="56">
         <v>42133</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="21">
-      <c r="A8" s="64" t="str">
-        <f>IF(OR(B8&lt;&gt;"",E8&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+      <c r="A8" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Add Customer-4]</v>
       </c>
-      <c r="B8" s="64" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="F8" s="62"/>
-      <c r="G8" s="61" t="s">
+      <c r="B8" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="58"/>
+      <c r="G8" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="60">
+      <c r="H8" s="56">
         <v>42133</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="21">
-      <c r="A9" s="64" t="str">
-        <f>IF(OR(B9&lt;&gt;"",E9&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+      <c r="A9" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Add Customer-5]</v>
       </c>
-      <c r="B9" s="64" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64" t="s">
-        <v>82</v>
-      </c>
-      <c r="E9" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="F9" s="62"/>
-      <c r="G9" s="61" t="s">
+      <c r="B9" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="58"/>
+      <c r="G9" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="60">
+      <c r="H9" s="56">
         <v>42133</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="21">
-      <c r="A10" s="64" t="str">
-        <f>IF(OR(B10&lt;&gt;"",E10&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+      <c r="A10" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Add Customer-6]</v>
       </c>
-      <c r="B10" s="64" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64" t="s">
-        <v>79</v>
-      </c>
-      <c r="E10" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="62"/>
-      <c r="G10" s="61" t="s">
+      <c r="B10" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="58"/>
+      <c r="G10" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="60">
+      <c r="H10" s="56">
         <v>42133</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="21">
-      <c r="A11" s="64" t="str">
-        <f>IF(OR(B11&lt;&gt;"",E11&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+      <c r="A11" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Add Customer-7]</v>
       </c>
-      <c r="B11" s="63" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="63" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="F11" s="62"/>
-      <c r="G11" s="61" t="s">
+      <c r="B11" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="58"/>
+      <c r="D11" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="58"/>
+      <c r="G11" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="60">
+      <c r="H11" s="56">
         <v>42133</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="21">
-      <c r="A12" s="64" t="str">
-        <f>IF(OR(B12&lt;&gt;"",E12&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+      <c r="A12" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Add Customer-8]</v>
       </c>
-      <c r="B12" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="62"/>
-      <c r="D12" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" s="62" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="62"/>
-      <c r="G12" s="61" t="s">
+      <c r="B12" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="58"/>
+      <c r="D12" s="59" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="58"/>
+      <c r="G12" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="60">
+      <c r="H12" s="56">
         <v>42133</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="31.5">
-      <c r="A13" s="64" t="str">
-        <f>IF(OR(B13&lt;&gt;"",E13&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+    <row r="13" spans="1:9" ht="21.75" customHeight="1">
+      <c r="A13" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Add Customer-9]</v>
       </c>
-      <c r="B13" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" s="62"/>
-      <c r="G13" s="61" t="s">
+      <c r="B13" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="58"/>
+      <c r="D13" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="58"/>
+      <c r="G13" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="60">
+      <c r="H13" s="56">
         <v>42133</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="31.5" customHeight="1">
-      <c r="A14" s="64" t="str">
-        <f>IF(OR(B14&lt;&gt;"",E14&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+    <row r="14" spans="1:9" ht="21.75" customHeight="1">
+      <c r="A14" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Add Customer-10]</v>
       </c>
-      <c r="B14" s="63" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="62" t="s">
-        <v>66</v>
-      </c>
-      <c r="F14" s="62"/>
-      <c r="G14" s="61" t="s">
+      <c r="B14" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="58"/>
+      <c r="D14" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="58"/>
+      <c r="G14" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="60">
+      <c r="H14" s="56">
         <v>42133</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="21.75" customHeight="1">
-      <c r="A15" s="64" t="str">
-        <f>IF(OR(B15&lt;&gt;"",E15&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+    <row r="15" spans="1:9" ht="21" customHeight="1">
+      <c r="A15" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Add Customer-11]</v>
       </c>
-      <c r="B15" s="63" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="63" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="62" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="62"/>
-      <c r="G15" s="61" t="s">
+      <c r="B15" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="58"/>
+      <c r="D15" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="58"/>
+      <c r="G15" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="60">
+      <c r="H15" s="56">
         <v>42133</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="21.75" customHeight="1">
-      <c r="A16" s="64" t="str">
-        <f>IF(OR(B16&lt;&gt;"",E16&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+      <c r="A16" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Add Customer-12]</v>
       </c>
-      <c r="B16" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" s="62"/>
-      <c r="G16" s="61" t="s">
+      <c r="B16" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="58"/>
+      <c r="D16" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="58"/>
+      <c r="G16" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="60">
+      <c r="H16" s="56">
         <v>42133</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="21" customHeight="1">
-      <c r="A17" s="64" t="str">
-        <f>IF(OR(B17&lt;&gt;"",E17&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
-        <v>[Add Customer-13]</v>
-      </c>
-      <c r="B17" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="62"/>
-      <c r="D17" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="62" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="62"/>
-      <c r="G17" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" s="60">
-        <v>42133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="21.75" customHeight="1">
-      <c r="A18" s="64" t="str">
-        <f>IF(OR(B18&lt;&gt;"",E18&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
-        <v>[Add Customer-14]</v>
-      </c>
-      <c r="B18" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="62" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="62"/>
-      <c r="G18" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="60">
-        <v>42133</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="10.5" customHeight="1"/>
-    <row r="20" spans="1:8" ht="10.5" customHeight="1"/>
-    <row r="21" spans="1:8" ht="10.5" customHeight="1"/>
-    <row r="22" spans="1:8" ht="10.5" customHeight="1"/>
-    <row r="23" spans="1:8" ht="10.5" customHeight="1"/>
-    <row r="24" spans="1:8" ht="10.5" customHeight="1"/>
-    <row r="25" spans="1:8" ht="10.5" customHeight="1"/>
-    <row r="26" spans="1:8" ht="10.5" customHeight="1"/>
-    <row r="27" spans="1:8" ht="10.5" customHeight="1"/>
-    <row r="28" spans="1:8" ht="10.5" customHeight="1"/>
-    <row r="29" spans="1:8" ht="10.5" customHeight="1"/>
-    <row r="30" spans="1:8" ht="10.5" customHeight="1"/>
-    <row r="31" spans="1:8" ht="10.5" customHeight="1"/>
-    <row r="32" spans="1:8" ht="10.5" customHeight="1"/>
+    <row r="17" ht="10.5" customHeight="1"/>
+    <row r="18" ht="10.5" customHeight="1"/>
+    <row r="19" ht="10.5" customHeight="1"/>
+    <row r="20" ht="10.5" customHeight="1"/>
+    <row r="21" ht="10.5" customHeight="1"/>
+    <row r="22" ht="10.5" customHeight="1"/>
+    <row r="23" ht="10.5" customHeight="1"/>
+    <row r="24" ht="10.5" customHeight="1"/>
+    <row r="25" ht="10.5" customHeight="1"/>
+    <row r="26" ht="10.5" customHeight="1"/>
+    <row r="27" ht="10.5" customHeight="1"/>
+    <row r="28" ht="10.5" customHeight="1"/>
+    <row r="29" ht="10.5" customHeight="1"/>
+    <row r="30" ht="10.5" customHeight="1"/>
+    <row r="31" ht="10.5" customHeight="1"/>
+    <row r="32" ht="10.5" customHeight="1"/>
     <row r="33" ht="10.5" customHeight="1"/>
     <row r="34" ht="10.5" customHeight="1"/>
     <row r="35" ht="10.5" customHeight="1"/>
@@ -3697,357 +3632,355 @@
     <row r="53" spans="2:2" ht="10.5" customHeight="1"/>
     <row r="54" spans="2:2" ht="10.5" customHeight="1"/>
     <row r="55" spans="2:2" ht="10.5" customHeight="1"/>
-    <row r="56" spans="2:2" ht="10.5" customHeight="1"/>
-    <row r="57" spans="2:2" ht="10.5" customHeight="1"/>
+    <row r="56" spans="2:2">
+      <c r="B56" s="55"/>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" s="55"/>
+    </row>
     <row r="58" spans="2:2">
-      <c r="B58" s="59"/>
+      <c r="B58" s="55"/>
     </row>
     <row r="59" spans="2:2">
-      <c r="B59" s="59"/>
+      <c r="B59" s="55"/>
     </row>
     <row r="60" spans="2:2">
-      <c r="B60" s="59"/>
+      <c r="B60" s="55"/>
     </row>
     <row r="61" spans="2:2">
-      <c r="B61" s="59"/>
+      <c r="B61" s="55"/>
     </row>
     <row r="62" spans="2:2">
-      <c r="B62" s="59"/>
+      <c r="B62" s="55"/>
     </row>
     <row r="63" spans="2:2">
-      <c r="B63" s="59"/>
+      <c r="B63" s="55"/>
     </row>
     <row r="64" spans="2:2">
-      <c r="B64" s="59"/>
+      <c r="B64" s="55"/>
     </row>
     <row r="65" spans="2:2">
-      <c r="B65" s="59"/>
+      <c r="B65" s="55"/>
     </row>
     <row r="66" spans="2:2">
-      <c r="B66" s="59"/>
+      <c r="B66" s="55"/>
     </row>
     <row r="67" spans="2:2">
-      <c r="B67" s="59"/>
+      <c r="B67" s="55"/>
     </row>
     <row r="68" spans="2:2">
-      <c r="B68" s="59"/>
+      <c r="B68" s="55"/>
     </row>
     <row r="69" spans="2:2">
-      <c r="B69" s="59"/>
+      <c r="B69" s="55"/>
     </row>
     <row r="70" spans="2:2">
-      <c r="B70" s="59"/>
+      <c r="B70" s="55"/>
     </row>
     <row r="71" spans="2:2">
-      <c r="B71" s="59"/>
+      <c r="B71" s="55"/>
     </row>
     <row r="72" spans="2:2">
-      <c r="B72" s="59"/>
+      <c r="B72" s="55"/>
     </row>
     <row r="73" spans="2:2">
-      <c r="B73" s="59"/>
+      <c r="B73" s="55"/>
     </row>
     <row r="74" spans="2:2">
-      <c r="B74" s="59"/>
+      <c r="B74" s="55"/>
     </row>
     <row r="75" spans="2:2">
-      <c r="B75" s="59"/>
+      <c r="B75" s="55"/>
     </row>
     <row r="76" spans="2:2">
-      <c r="B76" s="59"/>
+      <c r="B76" s="55"/>
     </row>
     <row r="77" spans="2:2">
-      <c r="B77" s="59"/>
+      <c r="B77" s="55"/>
     </row>
     <row r="78" spans="2:2">
-      <c r="B78" s="59"/>
+      <c r="B78" s="55"/>
     </row>
     <row r="79" spans="2:2">
-      <c r="B79" s="59"/>
+      <c r="B79" s="55"/>
     </row>
     <row r="80" spans="2:2">
-      <c r="B80" s="59"/>
+      <c r="B80" s="55"/>
     </row>
     <row r="81" spans="2:2">
-      <c r="B81" s="59"/>
+      <c r="B81" s="55"/>
     </row>
     <row r="82" spans="2:2">
-      <c r="B82" s="59"/>
+      <c r="B82" s="55"/>
     </row>
     <row r="83" spans="2:2">
-      <c r="B83" s="59"/>
+      <c r="B83" s="55"/>
     </row>
     <row r="84" spans="2:2">
-      <c r="B84" s="59"/>
+      <c r="B84" s="55"/>
     </row>
     <row r="85" spans="2:2">
-      <c r="B85" s="59"/>
+      <c r="B85" s="55"/>
     </row>
     <row r="86" spans="2:2">
-      <c r="B86" s="59"/>
+      <c r="B86" s="55"/>
     </row>
     <row r="87" spans="2:2">
-      <c r="B87" s="59"/>
+      <c r="B87" s="55"/>
     </row>
     <row r="88" spans="2:2">
-      <c r="B88" s="59"/>
+      <c r="B88" s="55"/>
     </row>
     <row r="89" spans="2:2">
-      <c r="B89" s="59"/>
+      <c r="B89" s="55"/>
     </row>
     <row r="90" spans="2:2">
-      <c r="B90" s="59"/>
+      <c r="B90" s="55"/>
     </row>
     <row r="91" spans="2:2">
-      <c r="B91" s="59"/>
+      <c r="B91" s="55"/>
     </row>
     <row r="92" spans="2:2">
-      <c r="B92" s="59"/>
+      <c r="B92" s="55"/>
     </row>
     <row r="93" spans="2:2">
-      <c r="B93" s="59"/>
+      <c r="B93" s="55"/>
     </row>
     <row r="94" spans="2:2">
-      <c r="B94" s="59"/>
+      <c r="B94" s="55"/>
     </row>
     <row r="95" spans="2:2">
-      <c r="B95" s="59"/>
+      <c r="B95" s="55"/>
     </row>
     <row r="96" spans="2:2">
-      <c r="B96" s="59"/>
+      <c r="B96" s="55"/>
     </row>
     <row r="97" spans="2:2">
-      <c r="B97" s="59"/>
+      <c r="B97" s="55"/>
     </row>
     <row r="98" spans="2:2">
-      <c r="B98" s="59"/>
+      <c r="B98" s="55"/>
     </row>
     <row r="99" spans="2:2">
-      <c r="B99" s="59"/>
+      <c r="B99" s="55"/>
     </row>
     <row r="100" spans="2:2">
-      <c r="B100" s="59"/>
+      <c r="B100" s="55"/>
     </row>
     <row r="101" spans="2:2">
-      <c r="B101" s="59"/>
+      <c r="B101" s="55"/>
     </row>
     <row r="102" spans="2:2">
-      <c r="B102" s="59"/>
+      <c r="B102" s="55"/>
     </row>
     <row r="103" spans="2:2">
-      <c r="B103" s="59"/>
+      <c r="B103" s="55"/>
     </row>
     <row r="104" spans="2:2">
-      <c r="B104" s="59"/>
+      <c r="B104" s="55"/>
     </row>
     <row r="105" spans="2:2">
-      <c r="B105" s="59"/>
+      <c r="B105" s="55"/>
     </row>
     <row r="106" spans="2:2">
-      <c r="B106" s="59"/>
+      <c r="B106" s="55"/>
     </row>
     <row r="107" spans="2:2">
-      <c r="B107" s="59"/>
+      <c r="B107" s="55"/>
     </row>
     <row r="108" spans="2:2">
-      <c r="B108" s="59"/>
+      <c r="B108" s="55"/>
     </row>
     <row r="109" spans="2:2">
-      <c r="B109" s="59"/>
+      <c r="B109" s="55"/>
     </row>
     <row r="110" spans="2:2">
-      <c r="B110" s="59"/>
+      <c r="B110" s="55"/>
     </row>
     <row r="111" spans="2:2">
-      <c r="B111" s="59"/>
+      <c r="B111" s="55"/>
     </row>
     <row r="112" spans="2:2">
-      <c r="B112" s="59"/>
+      <c r="B112" s="55"/>
     </row>
     <row r="113" spans="2:2">
-      <c r="B113" s="59"/>
+      <c r="B113" s="55"/>
     </row>
     <row r="114" spans="2:2">
-      <c r="B114" s="59"/>
+      <c r="B114" s="55"/>
     </row>
     <row r="115" spans="2:2">
-      <c r="B115" s="59"/>
+      <c r="B115" s="55"/>
     </row>
     <row r="116" spans="2:2">
-      <c r="B116" s="59"/>
+      <c r="B116" s="55"/>
     </row>
     <row r="117" spans="2:2">
-      <c r="B117" s="59"/>
+      <c r="B117" s="55"/>
     </row>
     <row r="118" spans="2:2">
-      <c r="B118" s="59"/>
+      <c r="B118" s="55"/>
     </row>
     <row r="119" spans="2:2">
-      <c r="B119" s="59"/>
+      <c r="B119" s="55"/>
     </row>
     <row r="120" spans="2:2">
-      <c r="B120" s="59"/>
+      <c r="B120" s="55"/>
     </row>
     <row r="121" spans="2:2">
-      <c r="B121" s="59"/>
+      <c r="B121" s="55"/>
     </row>
     <row r="122" spans="2:2">
-      <c r="B122" s="59"/>
+      <c r="B122" s="55"/>
     </row>
     <row r="123" spans="2:2">
-      <c r="B123" s="59"/>
+      <c r="B123" s="55"/>
     </row>
     <row r="124" spans="2:2">
-      <c r="B124" s="59"/>
+      <c r="B124" s="55"/>
     </row>
     <row r="125" spans="2:2">
-      <c r="B125" s="59"/>
+      <c r="B125" s="55"/>
     </row>
     <row r="126" spans="2:2">
-      <c r="B126" s="59"/>
+      <c r="B126" s="55"/>
     </row>
     <row r="127" spans="2:2">
-      <c r="B127" s="59"/>
+      <c r="B127" s="55"/>
     </row>
     <row r="128" spans="2:2">
-      <c r="B128" s="59"/>
+      <c r="B128" s="55"/>
     </row>
     <row r="129" spans="2:2">
-      <c r="B129" s="59"/>
+      <c r="B129" s="55"/>
     </row>
     <row r="130" spans="2:2">
-      <c r="B130" s="59"/>
+      <c r="B130" s="55"/>
     </row>
     <row r="131" spans="2:2">
-      <c r="B131" s="59"/>
+      <c r="B131" s="55"/>
     </row>
     <row r="132" spans="2:2">
-      <c r="B132" s="59"/>
+      <c r="B132" s="55"/>
     </row>
     <row r="133" spans="2:2">
-      <c r="B133" s="59"/>
+      <c r="B133" s="55"/>
     </row>
     <row r="134" spans="2:2">
-      <c r="B134" s="59"/>
+      <c r="B134" s="55"/>
     </row>
     <row r="135" spans="2:2">
-      <c r="B135" s="59"/>
+      <c r="B135" s="55"/>
     </row>
     <row r="136" spans="2:2">
-      <c r="B136" s="59"/>
+      <c r="B136" s="55"/>
     </row>
     <row r="137" spans="2:2">
-      <c r="B137" s="59"/>
+      <c r="B137" s="55"/>
     </row>
     <row r="138" spans="2:2">
-      <c r="B138" s="59"/>
+      <c r="B138" s="55"/>
     </row>
     <row r="139" spans="2:2">
-      <c r="B139" s="59"/>
+      <c r="B139" s="55"/>
     </row>
     <row r="140" spans="2:2">
-      <c r="B140" s="59"/>
+      <c r="B140" s="55"/>
     </row>
     <row r="141" spans="2:2">
-      <c r="B141" s="59"/>
+      <c r="B141" s="55"/>
     </row>
     <row r="142" spans="2:2">
-      <c r="B142" s="59"/>
+      <c r="B142" s="55"/>
     </row>
     <row r="143" spans="2:2">
-      <c r="B143" s="59"/>
+      <c r="B143" s="55"/>
     </row>
     <row r="144" spans="2:2">
-      <c r="B144" s="59"/>
+      <c r="B144" s="55"/>
     </row>
     <row r="145" spans="2:2">
-      <c r="B145" s="59"/>
+      <c r="B145" s="55"/>
     </row>
     <row r="146" spans="2:2">
-      <c r="B146" s="59"/>
+      <c r="B146" s="55"/>
     </row>
     <row r="147" spans="2:2">
-      <c r="B147" s="59"/>
+      <c r="B147" s="55"/>
     </row>
     <row r="148" spans="2:2">
-      <c r="B148" s="59"/>
+      <c r="B148" s="55"/>
     </row>
     <row r="149" spans="2:2">
-      <c r="B149" s="59"/>
+      <c r="B149" s="55"/>
     </row>
     <row r="150" spans="2:2">
-      <c r="B150" s="59"/>
+      <c r="B150" s="55"/>
     </row>
     <row r="151" spans="2:2">
-      <c r="B151" s="59"/>
+      <c r="B151" s="55"/>
     </row>
     <row r="152" spans="2:2">
-      <c r="B152" s="59"/>
+      <c r="B152" s="55"/>
     </row>
     <row r="153" spans="2:2">
-      <c r="B153" s="59"/>
+      <c r="B153" s="55"/>
     </row>
     <row r="154" spans="2:2">
-      <c r="B154" s="59"/>
+      <c r="B154" s="55"/>
     </row>
     <row r="155" spans="2:2">
-      <c r="B155" s="59"/>
+      <c r="B155" s="55"/>
     </row>
     <row r="156" spans="2:2">
-      <c r="B156" s="59"/>
+      <c r="B156" s="55"/>
     </row>
     <row r="157" spans="2:2">
-      <c r="B157" s="59"/>
+      <c r="B157" s="55"/>
     </row>
     <row r="158" spans="2:2">
-      <c r="B158" s="59"/>
+      <c r="B158" s="55"/>
     </row>
     <row r="159" spans="2:2">
-      <c r="B159" s="59"/>
+      <c r="B159" s="55"/>
     </row>
     <row r="160" spans="2:2">
-      <c r="B160" s="59"/>
+      <c r="B160" s="55"/>
     </row>
     <row r="161" spans="2:2">
-      <c r="B161" s="59"/>
+      <c r="B161" s="55"/>
     </row>
     <row r="162" spans="2:2">
-      <c r="B162" s="59"/>
+      <c r="B162" s="55"/>
     </row>
     <row r="163" spans="2:2">
-      <c r="B163" s="59"/>
+      <c r="B163" s="55"/>
     </row>
     <row r="164" spans="2:2">
-      <c r="B164" s="59"/>
+      <c r="B164" s="55"/>
     </row>
     <row r="165" spans="2:2">
-      <c r="B165" s="59"/>
+      <c r="B165" s="55"/>
     </row>
     <row r="166" spans="2:2">
-      <c r="B166" s="59"/>
+      <c r="B166" s="55"/>
     </row>
     <row r="167" spans="2:2">
-      <c r="B167" s="59"/>
+      <c r="B167" s="55"/>
     </row>
     <row r="168" spans="2:2">
-      <c r="B168" s="59"/>
+      <c r="B168" s="55"/>
     </row>
     <row r="169" spans="2:2">
-      <c r="B169" s="59"/>
+      <c r="B169" s="55"/>
     </row>
     <row r="170" spans="2:2">
-      <c r="B170" s="59"/>
-    </row>
-    <row r="171" spans="2:2">
-      <c r="B171" s="59"/>
-    </row>
-    <row r="172" spans="2:2">
-      <c r="B172" s="59"/>
+      <c r="B170" s="55"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="G5:G18">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="G5:G16">
       <formula1>"Pass,Fail,Untest,N/A"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4067,263 +4000,263 @@
   <dimension ref="A1:I155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A18"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="58" customWidth="1"/>
-    <col min="2" max="2" width="32.875" style="58" customWidth="1"/>
-    <col min="3" max="3" width="14.25" style="58" customWidth="1"/>
-    <col min="4" max="4" width="39.875" style="58" customWidth="1"/>
-    <col min="5" max="5" width="37.25" style="58" customWidth="1"/>
-    <col min="6" max="6" width="10.5" style="58" customWidth="1"/>
-    <col min="7" max="7" width="11.875" style="58" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="58"/>
+    <col min="1" max="1" width="14.5" style="54" customWidth="1"/>
+    <col min="2" max="2" width="32.875" style="54" customWidth="1"/>
+    <col min="3" max="3" width="14.25" style="54" customWidth="1"/>
+    <col min="4" max="4" width="39.875" style="54" customWidth="1"/>
+    <col min="5" max="5" width="37.25" style="54" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="54" customWidth="1"/>
+    <col min="7" max="7" width="11.875" style="54" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="76"/>
+      <c r="C1" s="72"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="75"/>
+      <c r="F1" s="71"/>
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
     </row>
     <row r="2" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="74" t="s">
-        <v>116</v>
-      </c>
-      <c r="C2" s="73" t="str">
+      <c r="B2" s="70" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="69" t="str">
         <f>"Pass: "&amp;COUNTIF($G$5:$G$919,"Pass")</f>
         <v>Pass: 7</v>
       </c>
-      <c r="D2" s="73" t="str">
+      <c r="D2" s="69" t="str">
         <f>"Fail: "&amp;COUNTIF($G$5:$G$919,"Fail")</f>
         <v>Fail: 0</v>
       </c>
-      <c r="E2" s="71" t="str">
+      <c r="E2" s="67" t="str">
         <f>"N/A: "&amp;COUNTIF($G$5:$G$919,"N/A")</f>
         <v>N/A: 0</v>
       </c>
-      <c r="F2" s="71"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="62"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="58"/>
     </row>
     <row r="3" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="72" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="70" t="str">
+      <c r="B3" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="66" t="str">
         <f>"Number of cases: "&amp;(COUNTA($A$5:$A$919))</f>
         <v>Number of cases: 7</v>
       </c>
-      <c r="D3" s="71" t="str">
+      <c r="D3" s="67" t="str">
         <f>"Untested: "&amp;COUNTIF($G$5:$G$919,"Untest")</f>
         <v>Untested: 0</v>
       </c>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="62"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="58"/>
     </row>
     <row r="4" spans="1:9" ht="28.35" customHeight="1">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="67" t="s">
+      <c r="D4" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="67" t="s">
+      <c r="E4" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="68" t="s">
+      <c r="F4" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="63" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="63" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="21" customHeight="1">
+      <c r="A5" s="60" t="str">
+        <f t="shared" ref="A5:A11" si="0">IF(OR(B5&lt;&gt;"",E5&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+        <v>[Search Customer-1]</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="58"/>
+      <c r="D5" s="60" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="58" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="58"/>
+      <c r="G5" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="56">
+        <v>42133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="31.5">
+      <c r="A6" s="60" t="str">
+        <f t="shared" si="0"/>
+        <v>[Search Customer-2]</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="58"/>
+      <c r="D6" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="58"/>
+      <c r="G6" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="56">
+        <v>42133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="31.5">
+      <c r="A7" s="60" t="str">
+        <f t="shared" si="0"/>
+        <v>[Search Customer-3]</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="58"/>
+      <c r="D7" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="G4" s="67" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="67" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="21" customHeight="1">
-      <c r="A5" s="64" t="str">
-        <f>IF(OR(B5&lt;&gt;"",E5&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
-        <v>[Search Customer-1]</v>
-      </c>
-      <c r="B5" s="63" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="64" t="s">
-        <v>114</v>
-      </c>
-      <c r="E5" s="62" t="s">
-        <v>113</v>
-      </c>
-      <c r="F5" s="62"/>
-      <c r="G5" s="61" t="s">
+      <c r="F7" s="58"/>
+      <c r="G7" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="60">
+      <c r="H7" s="56">
         <v>42133</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="31.5">
-      <c r="A6" s="64" t="str">
-        <f>IF(OR(B6&lt;&gt;"",E6&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
-        <v>[Search Customer-2]</v>
-      </c>
-      <c r="B6" s="63" t="s">
-        <v>112</v>
-      </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="64" t="s">
-        <v>109</v>
-      </c>
-      <c r="E6" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="F6" s="62"/>
-      <c r="G6" s="61" t="s">
+    <row r="8" spans="1:9" ht="10.5" customHeight="1">
+      <c r="A8" s="60" t="str">
+        <f t="shared" si="0"/>
+        <v>[Search Customer-4]</v>
+      </c>
+      <c r="B8" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="58"/>
+      <c r="D8" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="58" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="58"/>
+      <c r="G8" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="60">
+      <c r="H8" s="56">
         <v>42133</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="31.5">
-      <c r="A7" s="64" t="str">
-        <f>IF(OR(B7&lt;&gt;"",E7&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
-        <v>[Search Customer-3]</v>
-      </c>
-      <c r="B7" s="63" t="s">
-        <v>110</v>
-      </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="64" t="s">
-        <v>109</v>
-      </c>
-      <c r="E7" s="62" t="s">
-        <v>100</v>
-      </c>
-      <c r="F7" s="62"/>
-      <c r="G7" s="61" t="s">
+    <row r="9" spans="1:9" ht="10.5" customHeight="1">
+      <c r="A9" s="60" t="str">
+        <f t="shared" si="0"/>
+        <v>[Search Customer-5]</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="58"/>
+      <c r="D9" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="58"/>
+      <c r="G9" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="60">
+      <c r="H9" s="56">
         <v>42133</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="10.5" customHeight="1">
-      <c r="A8" s="64" t="str">
-        <f>IF(OR(B8&lt;&gt;"",E8&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
-        <v>[Search Customer-4]</v>
-      </c>
-      <c r="B8" s="63" t="s">
-        <v>108</v>
-      </c>
-      <c r="C8" s="62"/>
-      <c r="D8" s="63" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" s="62" t="s">
-        <v>106</v>
-      </c>
-      <c r="F8" s="62"/>
-      <c r="G8" s="61" t="s">
+    <row r="10" spans="1:9" ht="10.5" customHeight="1">
+      <c r="A10" s="60" t="str">
+        <f t="shared" si="0"/>
+        <v>[Search Customer-6]</v>
+      </c>
+      <c r="B10" s="59" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="58"/>
+      <c r="D10" s="59" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="58"/>
+      <c r="G10" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="60">
+      <c r="H10" s="56">
         <v>42133</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="10.5" customHeight="1">
-      <c r="A9" s="64" t="str">
-        <f>IF(OR(B9&lt;&gt;"",E9&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
-        <v>[Search Customer-5]</v>
-      </c>
-      <c r="B9" s="63" t="s">
-        <v>105</v>
-      </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="63" t="s">
-        <v>104</v>
-      </c>
-      <c r="E9" s="62" t="s">
-        <v>103</v>
-      </c>
-      <c r="F9" s="62"/>
-      <c r="G9" s="61" t="s">
+    <row r="11" spans="1:9" ht="10.5" customHeight="1">
+      <c r="A11" s="60" t="str">
+        <f t="shared" si="0"/>
+        <v>[Search Customer-7]</v>
+      </c>
+      <c r="B11" s="59" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="58"/>
+      <c r="D11" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" s="58"/>
+      <c r="G11" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="60">
-        <v>42133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="10.5" customHeight="1">
-      <c r="A10" s="64" t="str">
-        <f>IF(OR(B10&lt;&gt;"",E10&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
-        <v>[Search Customer-6]</v>
-      </c>
-      <c r="B10" s="63" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="63" t="s">
-        <v>101</v>
-      </c>
-      <c r="E10" s="62" t="s">
-        <v>100</v>
-      </c>
-      <c r="F10" s="62"/>
-      <c r="G10" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="60">
-        <v>42133</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="10.5" customHeight="1">
-      <c r="A11" s="64" t="str">
-        <f>IF(OR(B11&lt;&gt;"",E11&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
-        <v>[Search Customer-7]</v>
-      </c>
-      <c r="B11" s="63" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="63" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" s="62" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" s="62"/>
-      <c r="G11" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="60">
+      <c r="H11" s="56">
         <v>42133</v>
       </c>
     </row>
@@ -4357,349 +4290,349 @@
     <row r="39" spans="2:2" ht="10.5" customHeight="1"/>
     <row r="40" spans="2:2" ht="10.5" customHeight="1"/>
     <row r="41" spans="2:2">
-      <c r="B41" s="59"/>
+      <c r="B41" s="55"/>
     </row>
     <row r="42" spans="2:2">
-      <c r="B42" s="59"/>
+      <c r="B42" s="55"/>
     </row>
     <row r="43" spans="2:2">
-      <c r="B43" s="59"/>
+      <c r="B43" s="55"/>
     </row>
     <row r="44" spans="2:2">
-      <c r="B44" s="59"/>
+      <c r="B44" s="55"/>
     </row>
     <row r="45" spans="2:2">
-      <c r="B45" s="59"/>
+      <c r="B45" s="55"/>
     </row>
     <row r="46" spans="2:2">
-      <c r="B46" s="59"/>
+      <c r="B46" s="55"/>
     </row>
     <row r="47" spans="2:2">
-      <c r="B47" s="59"/>
+      <c r="B47" s="55"/>
     </row>
     <row r="48" spans="2:2">
-      <c r="B48" s="59"/>
+      <c r="B48" s="55"/>
     </row>
     <row r="49" spans="2:2">
-      <c r="B49" s="59"/>
+      <c r="B49" s="55"/>
     </row>
     <row r="50" spans="2:2">
-      <c r="B50" s="59"/>
+      <c r="B50" s="55"/>
     </row>
     <row r="51" spans="2:2">
-      <c r="B51" s="59"/>
+      <c r="B51" s="55"/>
     </row>
     <row r="52" spans="2:2">
-      <c r="B52" s="59"/>
+      <c r="B52" s="55"/>
     </row>
     <row r="53" spans="2:2">
-      <c r="B53" s="59"/>
+      <c r="B53" s="55"/>
     </row>
     <row r="54" spans="2:2">
-      <c r="B54" s="59"/>
+      <c r="B54" s="55"/>
     </row>
     <row r="55" spans="2:2">
-      <c r="B55" s="59"/>
+      <c r="B55" s="55"/>
     </row>
     <row r="56" spans="2:2">
-      <c r="B56" s="59"/>
+      <c r="B56" s="55"/>
     </row>
     <row r="57" spans="2:2">
-      <c r="B57" s="59"/>
+      <c r="B57" s="55"/>
     </row>
     <row r="58" spans="2:2">
-      <c r="B58" s="59"/>
+      <c r="B58" s="55"/>
     </row>
     <row r="59" spans="2:2">
-      <c r="B59" s="59"/>
+      <c r="B59" s="55"/>
     </row>
     <row r="60" spans="2:2">
-      <c r="B60" s="59"/>
+      <c r="B60" s="55"/>
     </row>
     <row r="61" spans="2:2">
-      <c r="B61" s="59"/>
+      <c r="B61" s="55"/>
     </row>
     <row r="62" spans="2:2">
-      <c r="B62" s="59"/>
+      <c r="B62" s="55"/>
     </row>
     <row r="63" spans="2:2">
-      <c r="B63" s="59"/>
+      <c r="B63" s="55"/>
     </row>
     <row r="64" spans="2:2">
-      <c r="B64" s="59"/>
+      <c r="B64" s="55"/>
     </row>
     <row r="65" spans="2:2">
-      <c r="B65" s="59"/>
+      <c r="B65" s="55"/>
     </row>
     <row r="66" spans="2:2">
-      <c r="B66" s="59"/>
+      <c r="B66" s="55"/>
     </row>
     <row r="67" spans="2:2">
-      <c r="B67" s="59"/>
+      <c r="B67" s="55"/>
     </row>
     <row r="68" spans="2:2">
-      <c r="B68" s="59"/>
+      <c r="B68" s="55"/>
     </row>
     <row r="69" spans="2:2">
-      <c r="B69" s="59"/>
+      <c r="B69" s="55"/>
     </row>
     <row r="70" spans="2:2">
-      <c r="B70" s="59"/>
+      <c r="B70" s="55"/>
     </row>
     <row r="71" spans="2:2">
-      <c r="B71" s="59"/>
+      <c r="B71" s="55"/>
     </row>
     <row r="72" spans="2:2">
-      <c r="B72" s="59"/>
+      <c r="B72" s="55"/>
     </row>
     <row r="73" spans="2:2">
-      <c r="B73" s="59"/>
+      <c r="B73" s="55"/>
     </row>
     <row r="74" spans="2:2">
-      <c r="B74" s="59"/>
+      <c r="B74" s="55"/>
     </row>
     <row r="75" spans="2:2">
-      <c r="B75" s="59"/>
+      <c r="B75" s="55"/>
     </row>
     <row r="76" spans="2:2">
-      <c r="B76" s="59"/>
+      <c r="B76" s="55"/>
     </row>
     <row r="77" spans="2:2">
-      <c r="B77" s="59"/>
+      <c r="B77" s="55"/>
     </row>
     <row r="78" spans="2:2">
-      <c r="B78" s="59"/>
+      <c r="B78" s="55"/>
     </row>
     <row r="79" spans="2:2">
-      <c r="B79" s="59"/>
+      <c r="B79" s="55"/>
     </row>
     <row r="80" spans="2:2">
-      <c r="B80" s="59"/>
+      <c r="B80" s="55"/>
     </row>
     <row r="81" spans="2:2">
-      <c r="B81" s="59"/>
+      <c r="B81" s="55"/>
     </row>
     <row r="82" spans="2:2">
-      <c r="B82" s="59"/>
+      <c r="B82" s="55"/>
     </row>
     <row r="83" spans="2:2">
-      <c r="B83" s="59"/>
+      <c r="B83" s="55"/>
     </row>
     <row r="84" spans="2:2">
-      <c r="B84" s="59"/>
+      <c r="B84" s="55"/>
     </row>
     <row r="85" spans="2:2">
-      <c r="B85" s="59"/>
+      <c r="B85" s="55"/>
     </row>
     <row r="86" spans="2:2">
-      <c r="B86" s="59"/>
+      <c r="B86" s="55"/>
     </row>
     <row r="87" spans="2:2">
-      <c r="B87" s="59"/>
+      <c r="B87" s="55"/>
     </row>
     <row r="88" spans="2:2">
-      <c r="B88" s="59"/>
+      <c r="B88" s="55"/>
     </row>
     <row r="89" spans="2:2">
-      <c r="B89" s="59"/>
+      <c r="B89" s="55"/>
     </row>
     <row r="90" spans="2:2">
-      <c r="B90" s="59"/>
+      <c r="B90" s="55"/>
     </row>
     <row r="91" spans="2:2">
-      <c r="B91" s="59"/>
+      <c r="B91" s="55"/>
     </row>
     <row r="92" spans="2:2">
-      <c r="B92" s="59"/>
+      <c r="B92" s="55"/>
     </row>
     <row r="93" spans="2:2">
-      <c r="B93" s="59"/>
+      <c r="B93" s="55"/>
     </row>
     <row r="94" spans="2:2">
-      <c r="B94" s="59"/>
+      <c r="B94" s="55"/>
     </row>
     <row r="95" spans="2:2">
-      <c r="B95" s="59"/>
+      <c r="B95" s="55"/>
     </row>
     <row r="96" spans="2:2">
-      <c r="B96" s="59"/>
+      <c r="B96" s="55"/>
     </row>
     <row r="97" spans="2:2">
-      <c r="B97" s="59"/>
+      <c r="B97" s="55"/>
     </row>
     <row r="98" spans="2:2">
-      <c r="B98" s="59"/>
+      <c r="B98" s="55"/>
     </row>
     <row r="99" spans="2:2">
-      <c r="B99" s="59"/>
+      <c r="B99" s="55"/>
     </row>
     <row r="100" spans="2:2">
-      <c r="B100" s="59"/>
+      <c r="B100" s="55"/>
     </row>
     <row r="101" spans="2:2">
-      <c r="B101" s="59"/>
+      <c r="B101" s="55"/>
     </row>
     <row r="102" spans="2:2">
-      <c r="B102" s="59"/>
+      <c r="B102" s="55"/>
     </row>
     <row r="103" spans="2:2">
-      <c r="B103" s="59"/>
+      <c r="B103" s="55"/>
     </row>
     <row r="104" spans="2:2">
-      <c r="B104" s="59"/>
+      <c r="B104" s="55"/>
     </row>
     <row r="105" spans="2:2">
-      <c r="B105" s="59"/>
+      <c r="B105" s="55"/>
     </row>
     <row r="106" spans="2:2">
-      <c r="B106" s="59"/>
+      <c r="B106" s="55"/>
     </row>
     <row r="107" spans="2:2">
-      <c r="B107" s="59"/>
+      <c r="B107" s="55"/>
     </row>
     <row r="108" spans="2:2">
-      <c r="B108" s="59"/>
+      <c r="B108" s="55"/>
     </row>
     <row r="109" spans="2:2">
-      <c r="B109" s="59"/>
+      <c r="B109" s="55"/>
     </row>
     <row r="110" spans="2:2">
-      <c r="B110" s="59"/>
+      <c r="B110" s="55"/>
     </row>
     <row r="111" spans="2:2">
-      <c r="B111" s="59"/>
+      <c r="B111" s="55"/>
     </row>
     <row r="112" spans="2:2">
-      <c r="B112" s="59"/>
+      <c r="B112" s="55"/>
     </row>
     <row r="113" spans="2:2">
-      <c r="B113" s="59"/>
+      <c r="B113" s="55"/>
     </row>
     <row r="114" spans="2:2">
-      <c r="B114" s="59"/>
+      <c r="B114" s="55"/>
     </row>
     <row r="115" spans="2:2">
-      <c r="B115" s="59"/>
+      <c r="B115" s="55"/>
     </row>
     <row r="116" spans="2:2">
-      <c r="B116" s="59"/>
+      <c r="B116" s="55"/>
     </row>
     <row r="117" spans="2:2">
-      <c r="B117" s="59"/>
+      <c r="B117" s="55"/>
     </row>
     <row r="118" spans="2:2">
-      <c r="B118" s="59"/>
+      <c r="B118" s="55"/>
     </row>
     <row r="119" spans="2:2">
-      <c r="B119" s="59"/>
+      <c r="B119" s="55"/>
     </row>
     <row r="120" spans="2:2">
-      <c r="B120" s="59"/>
+      <c r="B120" s="55"/>
     </row>
     <row r="121" spans="2:2">
-      <c r="B121" s="59"/>
+      <c r="B121" s="55"/>
     </row>
     <row r="122" spans="2:2">
-      <c r="B122" s="59"/>
+      <c r="B122" s="55"/>
     </row>
     <row r="123" spans="2:2">
-      <c r="B123" s="59"/>
+      <c r="B123" s="55"/>
     </row>
     <row r="124" spans="2:2">
-      <c r="B124" s="59"/>
+      <c r="B124" s="55"/>
     </row>
     <row r="125" spans="2:2">
-      <c r="B125" s="59"/>
+      <c r="B125" s="55"/>
     </row>
     <row r="126" spans="2:2">
-      <c r="B126" s="59"/>
+      <c r="B126" s="55"/>
     </row>
     <row r="127" spans="2:2">
-      <c r="B127" s="59"/>
+      <c r="B127" s="55"/>
     </row>
     <row r="128" spans="2:2">
-      <c r="B128" s="59"/>
+      <c r="B128" s="55"/>
     </row>
     <row r="129" spans="2:2">
-      <c r="B129" s="59"/>
+      <c r="B129" s="55"/>
     </row>
     <row r="130" spans="2:2">
-      <c r="B130" s="59"/>
+      <c r="B130" s="55"/>
     </row>
     <row r="131" spans="2:2">
-      <c r="B131" s="59"/>
+      <c r="B131" s="55"/>
     </row>
     <row r="132" spans="2:2">
-      <c r="B132" s="59"/>
+      <c r="B132" s="55"/>
     </row>
     <row r="133" spans="2:2">
-      <c r="B133" s="59"/>
+      <c r="B133" s="55"/>
     </row>
     <row r="134" spans="2:2">
-      <c r="B134" s="59"/>
+      <c r="B134" s="55"/>
     </row>
     <row r="135" spans="2:2">
-      <c r="B135" s="59"/>
+      <c r="B135" s="55"/>
     </row>
     <row r="136" spans="2:2">
-      <c r="B136" s="59"/>
+      <c r="B136" s="55"/>
     </row>
     <row r="137" spans="2:2">
-      <c r="B137" s="59"/>
+      <c r="B137" s="55"/>
     </row>
     <row r="138" spans="2:2">
-      <c r="B138" s="59"/>
+      <c r="B138" s="55"/>
     </row>
     <row r="139" spans="2:2">
-      <c r="B139" s="59"/>
+      <c r="B139" s="55"/>
     </row>
     <row r="140" spans="2:2">
-      <c r="B140" s="59"/>
+      <c r="B140" s="55"/>
     </row>
     <row r="141" spans="2:2">
-      <c r="B141" s="59"/>
+      <c r="B141" s="55"/>
     </row>
     <row r="142" spans="2:2">
-      <c r="B142" s="59"/>
+      <c r="B142" s="55"/>
     </row>
     <row r="143" spans="2:2">
-      <c r="B143" s="59"/>
+      <c r="B143" s="55"/>
     </row>
     <row r="144" spans="2:2">
-      <c r="B144" s="59"/>
+      <c r="B144" s="55"/>
     </row>
     <row r="145" spans="2:2">
-      <c r="B145" s="59"/>
+      <c r="B145" s="55"/>
     </row>
     <row r="146" spans="2:2">
-      <c r="B146" s="59"/>
+      <c r="B146" s="55"/>
     </row>
     <row r="147" spans="2:2">
-      <c r="B147" s="59"/>
+      <c r="B147" s="55"/>
     </row>
     <row r="148" spans="2:2">
-      <c r="B148" s="59"/>
+      <c r="B148" s="55"/>
     </row>
     <row r="149" spans="2:2">
-      <c r="B149" s="59"/>
+      <c r="B149" s="55"/>
     </row>
     <row r="150" spans="2:2">
-      <c r="B150" s="59"/>
+      <c r="B150" s="55"/>
     </row>
     <row r="151" spans="2:2">
-      <c r="B151" s="59"/>
+      <c r="B151" s="55"/>
     </row>
     <row r="152" spans="2:2">
-      <c r="B152" s="59"/>
+      <c r="B152" s="55"/>
     </row>
     <row r="153" spans="2:2">
-      <c r="B153" s="59"/>
+      <c r="B153" s="55"/>
     </row>
     <row r="154" spans="2:2">
-      <c r="B154" s="59"/>
+      <c r="B154" s="55"/>
     </row>
     <row r="155" spans="2:2">
-      <c r="B155" s="59"/>
+      <c r="B155" s="55"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -4718,811 +4651,765 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I140"/>
+  <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="58" customWidth="1"/>
-    <col min="2" max="2" width="32.875" style="58" customWidth="1"/>
-    <col min="3" max="3" width="14.25" style="58" customWidth="1"/>
-    <col min="4" max="4" width="39.875" style="58" customWidth="1"/>
-    <col min="5" max="5" width="37.25" style="58" customWidth="1"/>
-    <col min="6" max="6" width="10.5" style="58" customWidth="1"/>
-    <col min="7" max="7" width="11.875" style="58" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="58"/>
+    <col min="1" max="1" width="14.5" style="54" customWidth="1"/>
+    <col min="2" max="2" width="32.875" style="54" customWidth="1"/>
+    <col min="3" max="3" width="14.25" style="54" customWidth="1"/>
+    <col min="4" max="4" width="39.875" style="54" customWidth="1"/>
+    <col min="5" max="5" width="37.25" style="54" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="54" customWidth="1"/>
+    <col min="7" max="7" width="11.875" style="54" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="76"/>
+      <c r="C1" s="72"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="75"/>
+      <c r="F1" s="71"/>
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
     </row>
     <row r="2" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="74" t="s">
-        <v>134</v>
-      </c>
-      <c r="C2" s="73" t="str">
-        <f>"Pass: "&amp;COUNTIF($G$5:$G$904,"Pass")</f>
-        <v>Pass: 15</v>
-      </c>
-      <c r="D2" s="73" t="str">
-        <f>"Fail: "&amp;COUNTIF($G$5:$G$904,"Fail")</f>
+      <c r="B2" s="70" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="69" t="str">
+        <f>"Pass: "&amp;COUNTIF($G$5:$G$902,"Pass")</f>
+        <v>Pass: 13</v>
+      </c>
+      <c r="D2" s="69" t="str">
+        <f>"Fail: "&amp;COUNTIF($G$5:$G$902,"Fail")</f>
         <v>Fail: 0</v>
       </c>
-      <c r="E2" s="71" t="str">
-        <f>"N/A: "&amp;COUNTIF($G$5:$G$904,"N/A")</f>
+      <c r="E2" s="67" t="str">
+        <f>"N/A: "&amp;COUNTIF($G$5:$G$902,"N/A")</f>
         <v>N/A: 0</v>
       </c>
-      <c r="F2" s="71"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="62"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="58"/>
     </row>
     <row r="3" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="72" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="70" t="str">
-        <f>"Number of cases: "&amp;(COUNTA($A$5:$A$904))</f>
-        <v>Number of cases: 15</v>
-      </c>
-      <c r="D3" s="71" t="str">
-        <f>"Untested: "&amp;COUNTIF($G$5:$G$904,"Untest")</f>
+      <c r="B3" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="66" t="str">
+        <f>"Number of cases: "&amp;(COUNTA($A$5:$A$902))</f>
+        <v>Number of cases: 13</v>
+      </c>
+      <c r="D3" s="67" t="str">
+        <f>"Untested: "&amp;COUNTIF($G$5:$G$902,"Untest")</f>
         <v>Untested: 0</v>
       </c>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="62"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="58"/>
     </row>
     <row r="4" spans="1:9" ht="28.35" customHeight="1">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="67" t="s">
+      <c r="D4" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="67" t="s">
+      <c r="E4" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="68" t="s">
-        <v>94</v>
-      </c>
-      <c r="G4" s="67" t="s">
+      <c r="F4" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="67" t="s">
+      <c r="H4" s="63" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="66" customFormat="1">
-      <c r="A5" s="64" t="str">
-        <f>IF(OR(B5&lt;&gt;"",E5&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+    <row r="5" spans="1:9" s="62" customFormat="1">
+      <c r="A5" s="60" t="str">
+        <f t="shared" ref="A5:A17" si="0">IF(OR(B5&lt;&gt;"",E5&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
         <v>[Update Customer-1]</v>
       </c>
-      <c r="B5" s="64" t="s">
-        <v>133</v>
-      </c>
-      <c r="C5" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" s="64" t="s">
-        <v>132</v>
-      </c>
-      <c r="E5" s="64" t="s">
-        <v>131</v>
-      </c>
-      <c r="F5" s="65"/>
-      <c r="G5" s="61" t="s">
+      <c r="B5" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="61"/>
+      <c r="G5" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="60">
+      <c r="H5" s="56">
         <v>42133</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="21">
-      <c r="A6" s="64" t="str">
-        <f>IF(OR(B6&lt;&gt;"",E6&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+      <c r="A6" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Update Customer-2]</v>
       </c>
-      <c r="B6" s="64" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="64" t="s">
-        <v>130</v>
-      </c>
-      <c r="E6" s="64" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="65"/>
-      <c r="G6" s="61" t="s">
+      <c r="B6" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="60" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="61"/>
+      <c r="G6" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="60">
+      <c r="H6" s="56">
         <v>42133</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="21">
-      <c r="A7" s="64" t="str">
-        <f>IF(OR(B7&lt;&gt;"",E7&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+      <c r="A7" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Update Customer-3]</v>
       </c>
-      <c r="B7" s="64" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="E7" s="64" t="s">
-        <v>87</v>
-      </c>
-      <c r="F7" s="65"/>
-      <c r="G7" s="61" t="s">
+      <c r="B7" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="61"/>
+      <c r="G7" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="60">
+      <c r="H7" s="56">
         <v>42133</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="21">
-      <c r="A8" s="64" t="str">
-        <f>IF(OR(B8&lt;&gt;"",E8&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+      <c r="A8" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Update Customer-4]</v>
       </c>
-      <c r="B8" s="64" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64" t="s">
-        <v>128</v>
-      </c>
-      <c r="E8" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="F8" s="65"/>
-      <c r="G8" s="61" t="s">
+      <c r="B8" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="61"/>
+      <c r="G8" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="60">
+      <c r="H8" s="56">
         <v>42133</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="21">
-      <c r="A9" s="64" t="str">
-        <f>IF(OR(B9&lt;&gt;"",E9&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+      <c r="A9" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Update Customer-5]</v>
       </c>
-      <c r="B9" s="64" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64" t="s">
-        <v>127</v>
-      </c>
-      <c r="E9" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="F9" s="62"/>
-      <c r="G9" s="61" t="s">
+      <c r="B9" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="E9" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="58"/>
+      <c r="G9" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="60">
+      <c r="H9" s="56">
         <v>42133</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="21">
-      <c r="A10" s="64" t="str">
-        <f>IF(OR(B10&lt;&gt;"",E10&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+      <c r="A10" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Update Customer-6]</v>
       </c>
-      <c r="B10" s="64" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64" t="s">
-        <v>127</v>
-      </c>
-      <c r="E10" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="62"/>
-      <c r="G10" s="61" t="s">
+      <c r="B10" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="58"/>
+      <c r="G10" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="60">
+      <c r="H10" s="56">
         <v>42133</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="21">
-      <c r="A11" s="64" t="str">
-        <f>IF(OR(B11&lt;&gt;"",E11&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+      <c r="A11" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Update Customer-7]</v>
       </c>
-      <c r="B11" s="64" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="F11" s="62"/>
-      <c r="G11" s="61" t="s">
+      <c r="B11" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="58"/>
+      <c r="G11" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="60">
+      <c r="H11" s="56">
         <v>42133</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="21">
-      <c r="A12" s="64" t="str">
-        <f>IF(OR(B12&lt;&gt;"",E12&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+      <c r="A12" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Update Customer-8]</v>
       </c>
-      <c r="B12" s="63" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="62"/>
-      <c r="D12" s="63" t="s">
-        <v>125</v>
-      </c>
-      <c r="E12" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="F12" s="62"/>
-      <c r="G12" s="61" t="s">
+      <c r="B12" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="58"/>
+      <c r="D12" s="59" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="58"/>
+      <c r="G12" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="60">
+      <c r="H12" s="56">
         <v>42133</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="21">
-      <c r="A13" s="64" t="str">
-        <f>IF(OR(B13&lt;&gt;"",E13&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+      <c r="A13" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Update Customer-9]</v>
       </c>
-      <c r="B13" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="63" t="s">
-        <v>124</v>
-      </c>
-      <c r="E13" s="62" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="62"/>
-      <c r="G13" s="61" t="s">
+      <c r="B13" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="58"/>
+      <c r="D13" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="58"/>
+      <c r="G13" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="60">
+      <c r="H13" s="56">
         <v>42133</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="31.5">
-      <c r="A14" s="64" t="str">
-        <f>IF(OR(B14&lt;&gt;"",E14&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+    <row r="14" spans="1:9" ht="21">
+      <c r="A14" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Update Customer-10]</v>
       </c>
-      <c r="B14" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="63" t="s">
-        <v>123</v>
-      </c>
-      <c r="E14" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" s="62"/>
-      <c r="G14" s="61" t="s">
+      <c r="B14" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="58"/>
+      <c r="D14" s="59" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="58"/>
+      <c r="G14" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="60">
+      <c r="H14" s="56">
         <v>42133</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="31.5">
-      <c r="A15" s="64" t="str">
-        <f>IF(OR(B15&lt;&gt;"",E15&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+    <row r="15" spans="1:9" ht="21">
+      <c r="A15" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Update Customer-11]</v>
       </c>
-      <c r="B15" s="63" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="63" t="s">
-        <v>122</v>
-      </c>
-      <c r="E15" s="62" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="62"/>
-      <c r="G15" s="61" t="s">
+      <c r="B15" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="58"/>
+      <c r="D15" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="58"/>
+      <c r="G15" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="60">
+      <c r="H15" s="56">
         <v>42133</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="21">
-      <c r="A16" s="64" t="str">
-        <f>IF(OR(B16&lt;&gt;"",E16&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+      <c r="A16" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Update Customer-12]</v>
       </c>
-      <c r="B16" s="63" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="63" t="s">
-        <v>121</v>
-      </c>
-      <c r="E16" s="62" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="62"/>
-      <c r="G16" s="61" t="s">
+      <c r="B16" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="58"/>
+      <c r="D16" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="E16" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" s="58"/>
+      <c r="G16" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="60">
+      <c r="H16" s="56">
         <v>42133</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="21">
-      <c r="A17" s="64" t="str">
-        <f>IF(OR(B17&lt;&gt;"",E17&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
+      <c r="A17" s="60" t="str">
+        <f t="shared" si="0"/>
         <v>[Update Customer-13]</v>
       </c>
-      <c r="B17" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="62"/>
-      <c r="D17" s="63" t="s">
-        <v>120</v>
-      </c>
-      <c r="E17" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="62"/>
-      <c r="G17" s="61" t="s">
+      <c r="B17" s="59" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="58"/>
+      <c r="D17" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="58"/>
+      <c r="G17" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="60">
+      <c r="H17" s="56">
         <v>42133</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="21">
-      <c r="A18" s="64" t="str">
-        <f>IF(OR(B18&lt;&gt;"",E18&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
-        <v>[Update Customer-14]</v>
-      </c>
-      <c r="B18" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="63" t="s">
-        <v>118</v>
-      </c>
-      <c r="E18" s="62" t="s">
-        <v>117</v>
-      </c>
-      <c r="F18" s="62"/>
-      <c r="G18" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="60">
-        <v>42133</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="21">
-      <c r="A19" s="64" t="str">
-        <f>IF(OR(B19&lt;&gt;"",E19&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
-        <v>[Update Customer-15]</v>
-      </c>
-      <c r="B19" s="63" t="s">
-        <v>119</v>
-      </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="63" t="s">
-        <v>118</v>
-      </c>
-      <c r="E19" s="62" t="s">
-        <v>117</v>
-      </c>
-      <c r="F19" s="62"/>
-      <c r="G19" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="60">
-        <v>42133</v>
-      </c>
-    </row>
+    <row r="18" spans="1:8" ht="10.5" customHeight="1"/>
+    <row r="19" spans="1:8" ht="10.5" customHeight="1"/>
     <row r="20" spans="1:8" ht="10.5" customHeight="1"/>
     <row r="21" spans="1:8" ht="10.5" customHeight="1"/>
     <row r="22" spans="1:8" ht="10.5" customHeight="1"/>
     <row r="23" spans="1:8" ht="10.5" customHeight="1"/>
-    <row r="24" spans="1:8" ht="10.5" customHeight="1"/>
-    <row r="25" spans="1:8" ht="10.5" customHeight="1"/>
+    <row r="24" spans="1:8">
+      <c r="B24" s="55"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="B25" s="55"/>
+    </row>
     <row r="26" spans="1:8">
-      <c r="B26" s="59"/>
+      <c r="B26" s="55"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="B27" s="59"/>
+      <c r="B27" s="55"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="B28" s="59"/>
+      <c r="B28" s="55"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="B29" s="59"/>
+      <c r="B29" s="55"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="B30" s="59"/>
+      <c r="B30" s="55"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="B31" s="59"/>
+      <c r="B31" s="55"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="B32" s="59"/>
+      <c r="B32" s="55"/>
     </row>
     <row r="33" spans="2:2">
-      <c r="B33" s="59"/>
+      <c r="B33" s="55"/>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="59"/>
+      <c r="B34" s="55"/>
     </row>
     <row r="35" spans="2:2">
-      <c r="B35" s="59"/>
+      <c r="B35" s="55"/>
     </row>
     <row r="36" spans="2:2">
-      <c r="B36" s="59"/>
+      <c r="B36" s="55"/>
     </row>
     <row r="37" spans="2:2">
-      <c r="B37" s="59"/>
+      <c r="B37" s="55"/>
     </row>
     <row r="38" spans="2:2">
-      <c r="B38" s="59"/>
+      <c r="B38" s="55"/>
     </row>
     <row r="39" spans="2:2">
-      <c r="B39" s="59"/>
+      <c r="B39" s="55"/>
     </row>
     <row r="40" spans="2:2">
-      <c r="B40" s="59"/>
+      <c r="B40" s="55"/>
     </row>
     <row r="41" spans="2:2">
-      <c r="B41" s="59"/>
+      <c r="B41" s="55"/>
     </row>
     <row r="42" spans="2:2">
-      <c r="B42" s="59"/>
+      <c r="B42" s="55"/>
     </row>
     <row r="43" spans="2:2">
-      <c r="B43" s="59"/>
+      <c r="B43" s="55"/>
     </row>
     <row r="44" spans="2:2">
-      <c r="B44" s="59"/>
+      <c r="B44" s="55"/>
     </row>
     <row r="45" spans="2:2">
-      <c r="B45" s="59"/>
+      <c r="B45" s="55"/>
     </row>
     <row r="46" spans="2:2">
-      <c r="B46" s="59"/>
+      <c r="B46" s="55"/>
     </row>
     <row r="47" spans="2:2">
-      <c r="B47" s="59"/>
+      <c r="B47" s="55"/>
     </row>
     <row r="48" spans="2:2">
-      <c r="B48" s="59"/>
+      <c r="B48" s="55"/>
     </row>
     <row r="49" spans="2:2">
-      <c r="B49" s="59"/>
+      <c r="B49" s="55"/>
     </row>
     <row r="50" spans="2:2">
-      <c r="B50" s="59"/>
+      <c r="B50" s="55"/>
     </row>
     <row r="51" spans="2:2">
-      <c r="B51" s="59"/>
+      <c r="B51" s="55"/>
     </row>
     <row r="52" spans="2:2">
-      <c r="B52" s="59"/>
+      <c r="B52" s="55"/>
     </row>
     <row r="53" spans="2:2">
-      <c r="B53" s="59"/>
+      <c r="B53" s="55"/>
     </row>
     <row r="54" spans="2:2">
-      <c r="B54" s="59"/>
+      <c r="B54" s="55"/>
     </row>
     <row r="55" spans="2:2">
-      <c r="B55" s="59"/>
+      <c r="B55" s="55"/>
     </row>
     <row r="56" spans="2:2">
-      <c r="B56" s="59"/>
+      <c r="B56" s="55"/>
     </row>
     <row r="57" spans="2:2">
-      <c r="B57" s="59"/>
+      <c r="B57" s="55"/>
     </row>
     <row r="58" spans="2:2">
-      <c r="B58" s="59"/>
+      <c r="B58" s="55"/>
     </row>
     <row r="59" spans="2:2">
-      <c r="B59" s="59"/>
+      <c r="B59" s="55"/>
     </row>
     <row r="60" spans="2:2">
-      <c r="B60" s="59"/>
+      <c r="B60" s="55"/>
     </row>
     <row r="61" spans="2:2">
-      <c r="B61" s="59"/>
+      <c r="B61" s="55"/>
     </row>
     <row r="62" spans="2:2">
-      <c r="B62" s="59"/>
+      <c r="B62" s="55"/>
     </row>
     <row r="63" spans="2:2">
-      <c r="B63" s="59"/>
+      <c r="B63" s="55"/>
     </row>
     <row r="64" spans="2:2">
-      <c r="B64" s="59"/>
+      <c r="B64" s="55"/>
     </row>
     <row r="65" spans="2:2">
-      <c r="B65" s="59"/>
+      <c r="B65" s="55"/>
     </row>
     <row r="66" spans="2:2">
-      <c r="B66" s="59"/>
+      <c r="B66" s="55"/>
     </row>
     <row r="67" spans="2:2">
-      <c r="B67" s="59"/>
+      <c r="B67" s="55"/>
     </row>
     <row r="68" spans="2:2">
-      <c r="B68" s="59"/>
+      <c r="B68" s="55"/>
     </row>
     <row r="69" spans="2:2">
-      <c r="B69" s="59"/>
+      <c r="B69" s="55"/>
     </row>
     <row r="70" spans="2:2">
-      <c r="B70" s="59"/>
+      <c r="B70" s="55"/>
     </row>
     <row r="71" spans="2:2">
-      <c r="B71" s="59"/>
+      <c r="B71" s="55"/>
     </row>
     <row r="72" spans="2:2">
-      <c r="B72" s="59"/>
+      <c r="B72" s="55"/>
     </row>
     <row r="73" spans="2:2">
-      <c r="B73" s="59"/>
+      <c r="B73" s="55"/>
     </row>
     <row r="74" spans="2:2">
-      <c r="B74" s="59"/>
+      <c r="B74" s="55"/>
     </row>
     <row r="75" spans="2:2">
-      <c r="B75" s="59"/>
+      <c r="B75" s="55"/>
     </row>
     <row r="76" spans="2:2">
-      <c r="B76" s="59"/>
+      <c r="B76" s="55"/>
     </row>
     <row r="77" spans="2:2">
-      <c r="B77" s="59"/>
+      <c r="B77" s="55"/>
     </row>
     <row r="78" spans="2:2">
-      <c r="B78" s="59"/>
+      <c r="B78" s="55"/>
     </row>
     <row r="79" spans="2:2">
-      <c r="B79" s="59"/>
+      <c r="B79" s="55"/>
     </row>
     <row r="80" spans="2:2">
-      <c r="B80" s="59"/>
+      <c r="B80" s="55"/>
     </row>
     <row r="81" spans="2:2">
-      <c r="B81" s="59"/>
+      <c r="B81" s="55"/>
     </row>
     <row r="82" spans="2:2">
-      <c r="B82" s="59"/>
+      <c r="B82" s="55"/>
     </row>
     <row r="83" spans="2:2">
-      <c r="B83" s="59"/>
+      <c r="B83" s="55"/>
     </row>
     <row r="84" spans="2:2">
-      <c r="B84" s="59"/>
+      <c r="B84" s="55"/>
     </row>
     <row r="85" spans="2:2">
-      <c r="B85" s="59"/>
+      <c r="B85" s="55"/>
     </row>
     <row r="86" spans="2:2">
-      <c r="B86" s="59"/>
+      <c r="B86" s="55"/>
     </row>
     <row r="87" spans="2:2">
-      <c r="B87" s="59"/>
+      <c r="B87" s="55"/>
     </row>
     <row r="88" spans="2:2">
-      <c r="B88" s="59"/>
+      <c r="B88" s="55"/>
     </row>
     <row r="89" spans="2:2">
-      <c r="B89" s="59"/>
+      <c r="B89" s="55"/>
     </row>
     <row r="90" spans="2:2">
-      <c r="B90" s="59"/>
+      <c r="B90" s="55"/>
     </row>
     <row r="91" spans="2:2">
-      <c r="B91" s="59"/>
+      <c r="B91" s="55"/>
     </row>
     <row r="92" spans="2:2">
-      <c r="B92" s="59"/>
+      <c r="B92" s="55"/>
     </row>
     <row r="93" spans="2:2">
-      <c r="B93" s="59"/>
+      <c r="B93" s="55"/>
     </row>
     <row r="94" spans="2:2">
-      <c r="B94" s="59"/>
+      <c r="B94" s="55"/>
     </row>
     <row r="95" spans="2:2">
-      <c r="B95" s="59"/>
+      <c r="B95" s="55"/>
     </row>
     <row r="96" spans="2:2">
-      <c r="B96" s="59"/>
+      <c r="B96" s="55"/>
     </row>
     <row r="97" spans="2:2">
-      <c r="B97" s="59"/>
+      <c r="B97" s="55"/>
     </row>
     <row r="98" spans="2:2">
-      <c r="B98" s="59"/>
+      <c r="B98" s="55"/>
     </row>
     <row r="99" spans="2:2">
-      <c r="B99" s="59"/>
+      <c r="B99" s="55"/>
     </row>
     <row r="100" spans="2:2">
-      <c r="B100" s="59"/>
+      <c r="B100" s="55"/>
     </row>
     <row r="101" spans="2:2">
-      <c r="B101" s="59"/>
+      <c r="B101" s="55"/>
     </row>
     <row r="102" spans="2:2">
-      <c r="B102" s="59"/>
+      <c r="B102" s="55"/>
     </row>
     <row r="103" spans="2:2">
-      <c r="B103" s="59"/>
+      <c r="B103" s="55"/>
     </row>
     <row r="104" spans="2:2">
-      <c r="B104" s="59"/>
+      <c r="B104" s="55"/>
     </row>
     <row r="105" spans="2:2">
-      <c r="B105" s="59"/>
+      <c r="B105" s="55"/>
     </row>
     <row r="106" spans="2:2">
-      <c r="B106" s="59"/>
+      <c r="B106" s="55"/>
     </row>
     <row r="107" spans="2:2">
-      <c r="B107" s="59"/>
+      <c r="B107" s="55"/>
     </row>
     <row r="108" spans="2:2">
-      <c r="B108" s="59"/>
+      <c r="B108" s="55"/>
     </row>
     <row r="109" spans="2:2">
-      <c r="B109" s="59"/>
+      <c r="B109" s="55"/>
     </row>
     <row r="110" spans="2:2">
-      <c r="B110" s="59"/>
+      <c r="B110" s="55"/>
     </row>
     <row r="111" spans="2:2">
-      <c r="B111" s="59"/>
+      <c r="B111" s="55"/>
     </row>
     <row r="112" spans="2:2">
-      <c r="B112" s="59"/>
+      <c r="B112" s="55"/>
     </row>
     <row r="113" spans="2:2">
-      <c r="B113" s="59"/>
+      <c r="B113" s="55"/>
     </row>
     <row r="114" spans="2:2">
-      <c r="B114" s="59"/>
+      <c r="B114" s="55"/>
     </row>
     <row r="115" spans="2:2">
-      <c r="B115" s="59"/>
+      <c r="B115" s="55"/>
     </row>
     <row r="116" spans="2:2">
-      <c r="B116" s="59"/>
+      <c r="B116" s="55"/>
     </row>
     <row r="117" spans="2:2">
-      <c r="B117" s="59"/>
+      <c r="B117" s="55"/>
     </row>
     <row r="118" spans="2:2">
-      <c r="B118" s="59"/>
+      <c r="B118" s="55"/>
     </row>
     <row r="119" spans="2:2">
-      <c r="B119" s="59"/>
+      <c r="B119" s="55"/>
     </row>
     <row r="120" spans="2:2">
-      <c r="B120" s="59"/>
+      <c r="B120" s="55"/>
     </row>
     <row r="121" spans="2:2">
-      <c r="B121" s="59"/>
+      <c r="B121" s="55"/>
     </row>
     <row r="122" spans="2:2">
-      <c r="B122" s="59"/>
+      <c r="B122" s="55"/>
     </row>
     <row r="123" spans="2:2">
-      <c r="B123" s="59"/>
+      <c r="B123" s="55"/>
     </row>
     <row r="124" spans="2:2">
-      <c r="B124" s="59"/>
+      <c r="B124" s="55"/>
     </row>
     <row r="125" spans="2:2">
-      <c r="B125" s="59"/>
+      <c r="B125" s="55"/>
     </row>
     <row r="126" spans="2:2">
-      <c r="B126" s="59"/>
+      <c r="B126" s="55"/>
     </row>
     <row r="127" spans="2:2">
-      <c r="B127" s="59"/>
+      <c r="B127" s="55"/>
     </row>
     <row r="128" spans="2:2">
-      <c r="B128" s="59"/>
+      <c r="B128" s="55"/>
     </row>
     <row r="129" spans="2:2">
-      <c r="B129" s="59"/>
+      <c r="B129" s="55"/>
     </row>
     <row r="130" spans="2:2">
-      <c r="B130" s="59"/>
+      <c r="B130" s="55"/>
     </row>
     <row r="131" spans="2:2">
-      <c r="B131" s="59"/>
+      <c r="B131" s="55"/>
     </row>
     <row r="132" spans="2:2">
-      <c r="B132" s="59"/>
+      <c r="B132" s="55"/>
     </row>
     <row r="133" spans="2:2">
-      <c r="B133" s="59"/>
+      <c r="B133" s="55"/>
     </row>
     <row r="134" spans="2:2">
-      <c r="B134" s="59"/>
+      <c r="B134" s="55"/>
     </row>
     <row r="135" spans="2:2">
-      <c r="B135" s="59"/>
+      <c r="B135" s="55"/>
     </row>
     <row r="136" spans="2:2">
-      <c r="B136" s="59"/>
+      <c r="B136" s="55"/>
     </row>
     <row r="137" spans="2:2">
-      <c r="B137" s="59"/>
+      <c r="B137" s="55"/>
     </row>
     <row r="138" spans="2:2">
-      <c r="B138" s="59"/>
-    </row>
-    <row r="139" spans="2:2">
-      <c r="B139" s="59"/>
-    </row>
-    <row r="140" spans="2:2">
-      <c r="B140" s="59"/>
+      <c r="B138" s="55"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="G5:G19">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="G5:G17">
       <formula1>"Pass,Fail,Untest,N/A"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5545,145 +5432,145 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="58" customWidth="1"/>
-    <col min="2" max="2" width="32.875" style="58" customWidth="1"/>
-    <col min="3" max="3" width="14.25" style="58" customWidth="1"/>
-    <col min="4" max="4" width="39.875" style="58" customWidth="1"/>
-    <col min="5" max="5" width="37.25" style="58" customWidth="1"/>
-    <col min="6" max="6" width="10.5" style="58" customWidth="1"/>
-    <col min="7" max="7" width="11.875" style="58" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="58"/>
+    <col min="1" max="1" width="14.5" style="54" customWidth="1"/>
+    <col min="2" max="2" width="32.875" style="54" customWidth="1"/>
+    <col min="3" max="3" width="14.25" style="54" customWidth="1"/>
+    <col min="4" max="4" width="39.875" style="54" customWidth="1"/>
+    <col min="5" max="5" width="37.25" style="54" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="54" customWidth="1"/>
+    <col min="7" max="7" width="11.875" style="54" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="76"/>
+      <c r="C1" s="72"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="75"/>
+      <c r="F1" s="71"/>
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
     </row>
     <row r="2" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="74" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="73" t="str">
+      <c r="B2" s="70" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="69" t="str">
         <f>"Pass: "&amp;COUNTIF($G$5:$G$904,"Pass")</f>
         <v>Pass: 2</v>
       </c>
-      <c r="D2" s="73" t="str">
+      <c r="D2" s="69" t="str">
         <f>"Fail: "&amp;COUNTIF($G$5:$G$904,"Fail")</f>
         <v>Fail: 0</v>
       </c>
-      <c r="E2" s="71" t="str">
+      <c r="E2" s="67" t="str">
         <f>"N/A: "&amp;COUNTIF($G$5:$G$904,"N/A")</f>
         <v>N/A: 0</v>
       </c>
-      <c r="F2" s="71"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="62"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="58"/>
     </row>
     <row r="3" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="72" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="70" t="str">
+      <c r="B3" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="66" t="str">
         <f>"Number of cases: "&amp;(COUNTA($A$5:$A$904))</f>
         <v>Number of cases: 2</v>
       </c>
-      <c r="D3" s="71" t="str">
+      <c r="D3" s="67" t="str">
         <f>"Untested: "&amp;COUNTIF($G$5:$G$904,"Untest")</f>
         <v>Untested: 0</v>
       </c>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="62"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="58"/>
     </row>
     <row r="4" spans="1:9" ht="28.35" customHeight="1">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="67" t="s">
+      <c r="D4" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="67" t="s">
+      <c r="E4" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="68" t="s">
-        <v>94</v>
-      </c>
-      <c r="G4" s="67" t="s">
+      <c r="F4" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="67" t="s">
+      <c r="H4" s="63" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="66" customFormat="1">
-      <c r="A5" s="64" t="str">
+    <row r="5" spans="1:9" s="62" customFormat="1">
+      <c r="A5" s="60" t="str">
         <f>IF(OR(B5&lt;&gt;"",E5&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
         <v>[Delete Customer-1]</v>
       </c>
-      <c r="B5" s="64" t="s">
-        <v>133</v>
-      </c>
-      <c r="C5" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" s="63" t="s">
-        <v>136</v>
-      </c>
-      <c r="E5" s="64" t="s">
-        <v>131</v>
-      </c>
-      <c r="F5" s="65"/>
-      <c r="G5" s="61" t="s">
+      <c r="B5" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="61"/>
+      <c r="G5" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="60">
+      <c r="H5" s="56">
         <v>42133</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="10.5" customHeight="1">
-      <c r="A6" s="64" t="str">
+      <c r="A6" s="60" t="str">
         <f>IF(OR(B6&lt;&gt;"",E6&lt;&gt;""),"["&amp;TEXT($B$2,"#")&amp;"-"&amp;TEXT(ROW()-4,"##")&amp;"]","")</f>
         <v>[Delete Customer-2]</v>
       </c>
-      <c r="B6" s="63" t="s">
-        <v>137</v>
-      </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="63" t="s">
-        <v>136</v>
-      </c>
-      <c r="E6" s="62" t="s">
-        <v>135</v>
-      </c>
-      <c r="F6" s="62"/>
-      <c r="G6" s="61" t="s">
+      <c r="B6" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="58"/>
+      <c r="D6" s="59" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="58"/>
+      <c r="G6" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="60">
+      <c r="H6" s="56">
         <v>42133</v>
       </c>
     </row>
@@ -5707,349 +5594,349 @@
     <row r="24" spans="2:2" ht="10.5" customHeight="1"/>
     <row r="25" spans="2:2" ht="10.5" customHeight="1"/>
     <row r="26" spans="2:2">
-      <c r="B26" s="59"/>
+      <c r="B26" s="55"/>
     </row>
     <row r="27" spans="2:2">
-      <c r="B27" s="59"/>
+      <c r="B27" s="55"/>
     </row>
     <row r="28" spans="2:2">
-      <c r="B28" s="59"/>
+      <c r="B28" s="55"/>
     </row>
     <row r="29" spans="2:2">
-      <c r="B29" s="59"/>
+      <c r="B29" s="55"/>
     </row>
     <row r="30" spans="2:2">
-      <c r="B30" s="59"/>
+      <c r="B30" s="55"/>
     </row>
     <row r="31" spans="2:2">
-      <c r="B31" s="59"/>
+      <c r="B31" s="55"/>
     </row>
     <row r="32" spans="2:2">
-      <c r="B32" s="59"/>
+      <c r="B32" s="55"/>
     </row>
     <row r="33" spans="2:2">
-      <c r="B33" s="59"/>
+      <c r="B33" s="55"/>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="59"/>
+      <c r="B34" s="55"/>
     </row>
     <row r="35" spans="2:2">
-      <c r="B35" s="59"/>
+      <c r="B35" s="55"/>
     </row>
     <row r="36" spans="2:2">
-      <c r="B36" s="59"/>
+      <c r="B36" s="55"/>
     </row>
     <row r="37" spans="2:2">
-      <c r="B37" s="59"/>
+      <c r="B37" s="55"/>
     </row>
     <row r="38" spans="2:2">
-      <c r="B38" s="59"/>
+      <c r="B38" s="55"/>
     </row>
     <row r="39" spans="2:2">
-      <c r="B39" s="59"/>
+      <c r="B39" s="55"/>
     </row>
     <row r="40" spans="2:2">
-      <c r="B40" s="59"/>
+      <c r="B40" s="55"/>
     </row>
     <row r="41" spans="2:2">
-      <c r="B41" s="59"/>
+      <c r="B41" s="55"/>
     </row>
     <row r="42" spans="2:2">
-      <c r="B42" s="59"/>
+      <c r="B42" s="55"/>
     </row>
     <row r="43" spans="2:2">
-      <c r="B43" s="59"/>
+      <c r="B43" s="55"/>
     </row>
     <row r="44" spans="2:2">
-      <c r="B44" s="59"/>
+      <c r="B44" s="55"/>
     </row>
     <row r="45" spans="2:2">
-      <c r="B45" s="59"/>
+      <c r="B45" s="55"/>
     </row>
     <row r="46" spans="2:2">
-      <c r="B46" s="59"/>
+      <c r="B46" s="55"/>
     </row>
     <row r="47" spans="2:2">
-      <c r="B47" s="59"/>
+      <c r="B47" s="55"/>
     </row>
     <row r="48" spans="2:2">
-      <c r="B48" s="59"/>
+      <c r="B48" s="55"/>
     </row>
     <row r="49" spans="2:2">
-      <c r="B49" s="59"/>
+      <c r="B49" s="55"/>
     </row>
     <row r="50" spans="2:2">
-      <c r="B50" s="59"/>
+      <c r="B50" s="55"/>
     </row>
     <row r="51" spans="2:2">
-      <c r="B51" s="59"/>
+      <c r="B51" s="55"/>
     </row>
     <row r="52" spans="2:2">
-      <c r="B52" s="59"/>
+      <c r="B52" s="55"/>
     </row>
     <row r="53" spans="2:2">
-      <c r="B53" s="59"/>
+      <c r="B53" s="55"/>
     </row>
     <row r="54" spans="2:2">
-      <c r="B54" s="59"/>
+      <c r="B54" s="55"/>
     </row>
     <row r="55" spans="2:2">
-      <c r="B55" s="59"/>
+      <c r="B55" s="55"/>
     </row>
     <row r="56" spans="2:2">
-      <c r="B56" s="59"/>
+      <c r="B56" s="55"/>
     </row>
     <row r="57" spans="2:2">
-      <c r="B57" s="59"/>
+      <c r="B57" s="55"/>
     </row>
     <row r="58" spans="2:2">
-      <c r="B58" s="59"/>
+      <c r="B58" s="55"/>
     </row>
     <row r="59" spans="2:2">
-      <c r="B59" s="59"/>
+      <c r="B59" s="55"/>
     </row>
     <row r="60" spans="2:2">
-      <c r="B60" s="59"/>
+      <c r="B60" s="55"/>
     </row>
     <row r="61" spans="2:2">
-      <c r="B61" s="59"/>
+      <c r="B61" s="55"/>
     </row>
     <row r="62" spans="2:2">
-      <c r="B62" s="59"/>
+      <c r="B62" s="55"/>
     </row>
     <row r="63" spans="2:2">
-      <c r="B63" s="59"/>
+      <c r="B63" s="55"/>
     </row>
     <row r="64" spans="2:2">
-      <c r="B64" s="59"/>
+      <c r="B64" s="55"/>
     </row>
     <row r="65" spans="2:2">
-      <c r="B65" s="59"/>
+      <c r="B65" s="55"/>
     </row>
     <row r="66" spans="2:2">
-      <c r="B66" s="59"/>
+      <c r="B66" s="55"/>
     </row>
     <row r="67" spans="2:2">
-      <c r="B67" s="59"/>
+      <c r="B67" s="55"/>
     </row>
     <row r="68" spans="2:2">
-      <c r="B68" s="59"/>
+      <c r="B68" s="55"/>
     </row>
     <row r="69" spans="2:2">
-      <c r="B69" s="59"/>
+      <c r="B69" s="55"/>
     </row>
     <row r="70" spans="2:2">
-      <c r="B70" s="59"/>
+      <c r="B70" s="55"/>
     </row>
     <row r="71" spans="2:2">
-      <c r="B71" s="59"/>
+      <c r="B71" s="55"/>
     </row>
     <row r="72" spans="2:2">
-      <c r="B72" s="59"/>
+      <c r="B72" s="55"/>
     </row>
     <row r="73" spans="2:2">
-      <c r="B73" s="59"/>
+      <c r="B73" s="55"/>
     </row>
     <row r="74" spans="2:2">
-      <c r="B74" s="59"/>
+      <c r="B74" s="55"/>
     </row>
     <row r="75" spans="2:2">
-      <c r="B75" s="59"/>
+      <c r="B75" s="55"/>
     </row>
     <row r="76" spans="2:2">
-      <c r="B76" s="59"/>
+      <c r="B76" s="55"/>
     </row>
     <row r="77" spans="2:2">
-      <c r="B77" s="59"/>
+      <c r="B77" s="55"/>
     </row>
     <row r="78" spans="2:2">
-      <c r="B78" s="59"/>
+      <c r="B78" s="55"/>
     </row>
     <row r="79" spans="2:2">
-      <c r="B79" s="59"/>
+      <c r="B79" s="55"/>
     </row>
     <row r="80" spans="2:2">
-      <c r="B80" s="59"/>
+      <c r="B80" s="55"/>
     </row>
     <row r="81" spans="2:2">
-      <c r="B81" s="59"/>
+      <c r="B81" s="55"/>
     </row>
     <row r="82" spans="2:2">
-      <c r="B82" s="59"/>
+      <c r="B82" s="55"/>
     </row>
     <row r="83" spans="2:2">
-      <c r="B83" s="59"/>
+      <c r="B83" s="55"/>
     </row>
     <row r="84" spans="2:2">
-      <c r="B84" s="59"/>
+      <c r="B84" s="55"/>
     </row>
     <row r="85" spans="2:2">
-      <c r="B85" s="59"/>
+      <c r="B85" s="55"/>
     </row>
     <row r="86" spans="2:2">
-      <c r="B86" s="59"/>
+      <c r="B86" s="55"/>
     </row>
     <row r="87" spans="2:2">
-      <c r="B87" s="59"/>
+      <c r="B87" s="55"/>
     </row>
     <row r="88" spans="2:2">
-      <c r="B88" s="59"/>
+      <c r="B88" s="55"/>
     </row>
     <row r="89" spans="2:2">
-      <c r="B89" s="59"/>
+      <c r="B89" s="55"/>
     </row>
     <row r="90" spans="2:2">
-      <c r="B90" s="59"/>
+      <c r="B90" s="55"/>
     </row>
     <row r="91" spans="2:2">
-      <c r="B91" s="59"/>
+      <c r="B91" s="55"/>
     </row>
     <row r="92" spans="2:2">
-      <c r="B92" s="59"/>
+      <c r="B92" s="55"/>
     </row>
     <row r="93" spans="2:2">
-      <c r="B93" s="59"/>
+      <c r="B93" s="55"/>
     </row>
     <row r="94" spans="2:2">
-      <c r="B94" s="59"/>
+      <c r="B94" s="55"/>
     </row>
     <row r="95" spans="2:2">
-      <c r="B95" s="59"/>
+      <c r="B95" s="55"/>
     </row>
     <row r="96" spans="2:2">
-      <c r="B96" s="59"/>
+      <c r="B96" s="55"/>
     </row>
     <row r="97" spans="2:2">
-      <c r="B97" s="59"/>
+      <c r="B97" s="55"/>
     </row>
     <row r="98" spans="2:2">
-      <c r="B98" s="59"/>
+      <c r="B98" s="55"/>
     </row>
     <row r="99" spans="2:2">
-      <c r="B99" s="59"/>
+      <c r="B99" s="55"/>
     </row>
     <row r="100" spans="2:2">
-      <c r="B100" s="59"/>
+      <c r="B100" s="55"/>
     </row>
     <row r="101" spans="2:2">
-      <c r="B101" s="59"/>
+      <c r="B101" s="55"/>
     </row>
     <row r="102" spans="2:2">
-      <c r="B102" s="59"/>
+      <c r="B102" s="55"/>
     </row>
     <row r="103" spans="2:2">
-      <c r="B103" s="59"/>
+      <c r="B103" s="55"/>
     </row>
     <row r="104" spans="2:2">
-      <c r="B104" s="59"/>
+      <c r="B104" s="55"/>
     </row>
     <row r="105" spans="2:2">
-      <c r="B105" s="59"/>
+      <c r="B105" s="55"/>
     </row>
     <row r="106" spans="2:2">
-      <c r="B106" s="59"/>
+      <c r="B106" s="55"/>
     </row>
     <row r="107" spans="2:2">
-      <c r="B107" s="59"/>
+      <c r="B107" s="55"/>
     </row>
     <row r="108" spans="2:2">
-      <c r="B108" s="59"/>
+      <c r="B108" s="55"/>
     </row>
     <row r="109" spans="2:2">
-      <c r="B109" s="59"/>
+      <c r="B109" s="55"/>
     </row>
     <row r="110" spans="2:2">
-      <c r="B110" s="59"/>
+      <c r="B110" s="55"/>
     </row>
     <row r="111" spans="2:2">
-      <c r="B111" s="59"/>
+      <c r="B111" s="55"/>
     </row>
     <row r="112" spans="2:2">
-      <c r="B112" s="59"/>
+      <c r="B112" s="55"/>
     </row>
     <row r="113" spans="2:2">
-      <c r="B113" s="59"/>
+      <c r="B113" s="55"/>
     </row>
     <row r="114" spans="2:2">
-      <c r="B114" s="59"/>
+      <c r="B114" s="55"/>
     </row>
     <row r="115" spans="2:2">
-      <c r="B115" s="59"/>
+      <c r="B115" s="55"/>
     </row>
     <row r="116" spans="2:2">
-      <c r="B116" s="59"/>
+      <c r="B116" s="55"/>
     </row>
     <row r="117" spans="2:2">
-      <c r="B117" s="59"/>
+      <c r="B117" s="55"/>
     </row>
     <row r="118" spans="2:2">
-      <c r="B118" s="59"/>
+      <c r="B118" s="55"/>
     </row>
     <row r="119" spans="2:2">
-      <c r="B119" s="59"/>
+      <c r="B119" s="55"/>
     </row>
     <row r="120" spans="2:2">
-      <c r="B120" s="59"/>
+      <c r="B120" s="55"/>
     </row>
     <row r="121" spans="2:2">
-      <c r="B121" s="59"/>
+      <c r="B121" s="55"/>
     </row>
     <row r="122" spans="2:2">
-      <c r="B122" s="59"/>
+      <c r="B122" s="55"/>
     </row>
     <row r="123" spans="2:2">
-      <c r="B123" s="59"/>
+      <c r="B123" s="55"/>
     </row>
     <row r="124" spans="2:2">
-      <c r="B124" s="59"/>
+      <c r="B124" s="55"/>
     </row>
     <row r="125" spans="2:2">
-      <c r="B125" s="59"/>
+      <c r="B125" s="55"/>
     </row>
     <row r="126" spans="2:2">
-      <c r="B126" s="59"/>
+      <c r="B126" s="55"/>
     </row>
     <row r="127" spans="2:2">
-      <c r="B127" s="59"/>
+      <c r="B127" s="55"/>
     </row>
     <row r="128" spans="2:2">
-      <c r="B128" s="59"/>
+      <c r="B128" s="55"/>
     </row>
     <row r="129" spans="2:2">
-      <c r="B129" s="59"/>
+      <c r="B129" s="55"/>
     </row>
     <row r="130" spans="2:2">
-      <c r="B130" s="59"/>
+      <c r="B130" s="55"/>
     </row>
     <row r="131" spans="2:2">
-      <c r="B131" s="59"/>
+      <c r="B131" s="55"/>
     </row>
     <row r="132" spans="2:2">
-      <c r="B132" s="59"/>
+      <c r="B132" s="55"/>
     </row>
     <row r="133" spans="2:2">
-      <c r="B133" s="59"/>
+      <c r="B133" s="55"/>
     </row>
     <row r="134" spans="2:2">
-      <c r="B134" s="59"/>
+      <c r="B134" s="55"/>
     </row>
     <row r="135" spans="2:2">
-      <c r="B135" s="59"/>
+      <c r="B135" s="55"/>
     </row>
     <row r="136" spans="2:2">
-      <c r="B136" s="59"/>
+      <c r="B136" s="55"/>
     </row>
     <row r="137" spans="2:2">
-      <c r="B137" s="59"/>
+      <c r="B137" s="55"/>
     </row>
     <row r="138" spans="2:2">
-      <c r="B138" s="59"/>
+      <c r="B138" s="55"/>
     </row>
     <row r="139" spans="2:2">
-      <c r="B139" s="59"/>
+      <c r="B139" s="55"/>
     </row>
     <row r="140" spans="2:2">
-      <c r="B140" s="59"/>
+      <c r="B140" s="55"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>